<commit_message>
First program integration and updates to the documents.
</commit_message>
<xml_diff>
--- a/ESTRUCTURA DEL PROYECTO/2) Planning/Gantt-Chart_SW_proyect.xlsx
+++ b/ESTRUCTURA DEL PROYECTO/2) Planning/Gantt-Chart_SW_proyect.xlsx
@@ -1,29 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SEI203\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Diplomado\Docs\proyecto\out\ceseq_diplomado-master\Proyecto_Integrador\ESTRUCTURA DEL PROYECTO\2) Planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{401F1857-986A-4144-A2C6-D27F337D1F96}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="285" yWindow="465" windowWidth="50925" windowHeight="27405"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-  </externalReferences>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="181029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="330"/>
     </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -33,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="41">
   <si>
     <t>Task 1</t>
   </si>
@@ -86,9 +89,6 @@
     <t>Task 17</t>
   </si>
   <si>
-    <t>Project Lead</t>
-  </si>
-  <si>
     <t>Phase 1</t>
   </si>
   <si>
@@ -131,9 +131,6 @@
     <t>PROJECT PLAN</t>
   </si>
   <si>
-    <t>SW DIPLOMA</t>
-  </si>
-  <si>
     <t xml:space="preserve">Delivery of complete proyect </t>
   </si>
   <si>
@@ -159,12 +156,15 @@
   </si>
   <si>
     <t>SW-Ports and pin configuration for timers and PWM.</t>
+  </si>
+  <si>
+    <t>Proyecto Integrador</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -348,7 +348,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="2" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -356,6 +355,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -402,7 +402,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -503,7 +502,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -795,7 +793,7 @@
                 <c:order val="1"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$D$5</c15:sqref>
@@ -822,7 +820,7 @@
                 <c:invertIfNegative val="0"/>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$D$6:$D$24</c15:sqref>
@@ -892,7 +890,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000005-9AED-451E-85E8-79C94647ABA1}"/>
                   </c:ext>
@@ -1021,7 +1019,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1650,7 +1647,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="17" name="Gráfico 16"/>
+        <xdr:cNvPr id="17" name="Gráfico 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000011000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1666,207 +1669,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Sheet1"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="6">
-          <cell r="A6" t="str">
-            <v>Task 1</v>
-          </cell>
-          <cell r="C6">
-            <v>43125</v>
-          </cell>
-          <cell r="E6">
-            <v>5</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="A7" t="str">
-            <v>Task 2</v>
-          </cell>
-          <cell r="C7">
-            <v>43125</v>
-          </cell>
-          <cell r="E7">
-            <v>7</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="A8" t="str">
-            <v>Task 3</v>
-          </cell>
-          <cell r="C8">
-            <v>43127</v>
-          </cell>
-          <cell r="E8">
-            <v>8</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="A9" t="str">
-            <v>Task 4</v>
-          </cell>
-          <cell r="C9">
-            <v>43129</v>
-          </cell>
-          <cell r="E9">
-            <v>8</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="A10" t="str">
-            <v>Task 5</v>
-          </cell>
-          <cell r="C10">
-            <v>43132</v>
-          </cell>
-          <cell r="E10">
-            <v>8</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="A11" t="str">
-            <v>Task 6</v>
-          </cell>
-          <cell r="C11">
-            <v>43132</v>
-          </cell>
-          <cell r="E11">
-            <v>4</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="A12" t="str">
-            <v>Task 7</v>
-          </cell>
-          <cell r="C12">
-            <v>43134</v>
-          </cell>
-          <cell r="E12">
-            <v>7</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="A13" t="str">
-            <v>Task 8</v>
-          </cell>
-          <cell r="C13">
-            <v>43136</v>
-          </cell>
-          <cell r="E13">
-            <v>7</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="A14" t="str">
-            <v>Task 9</v>
-          </cell>
-          <cell r="C14">
-            <v>43134</v>
-          </cell>
-          <cell r="E14">
-            <v>6</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="A15" t="str">
-            <v>Task 10</v>
-          </cell>
-          <cell r="C15">
-            <v>43137</v>
-          </cell>
-          <cell r="E15">
-            <v>4</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="A16" t="str">
-            <v>Task 11</v>
-          </cell>
-          <cell r="C16">
-            <v>43138</v>
-          </cell>
-          <cell r="E16">
-            <v>6</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="A17" t="str">
-            <v>Task 12</v>
-          </cell>
-          <cell r="C17">
-            <v>43141</v>
-          </cell>
-          <cell r="E17">
-            <v>6</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="A18" t="str">
-            <v>Task 13</v>
-          </cell>
-          <cell r="C18">
-            <v>43145</v>
-          </cell>
-          <cell r="E18">
-            <v>5</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="A19" t="str">
-            <v>Task 14</v>
-          </cell>
-          <cell r="C19">
-            <v>43146</v>
-          </cell>
-          <cell r="E19">
-            <v>8</v>
-          </cell>
-        </row>
-        <row r="20">
-          <cell r="A20" t="str">
-            <v>Task 15</v>
-          </cell>
-          <cell r="C20">
-            <v>43147</v>
-          </cell>
-          <cell r="E20">
-            <v>10</v>
-          </cell>
-        </row>
-        <row r="21">
-          <cell r="A21" t="str">
-            <v>Task 16</v>
-          </cell>
-          <cell r="C21">
-            <v>43151</v>
-          </cell>
-          <cell r="E21">
-            <v>8</v>
-          </cell>
-        </row>
-        <row r="22">
-          <cell r="A22" t="str">
-            <v>Task 17</v>
-          </cell>
-          <cell r="C22">
-            <v>43155</v>
-          </cell>
-          <cell r="E22">
-            <v>5</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2165,14 +1967,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor theme="4" tint="0.39997558519241921"/>
   </sheetPr>
   <dimension ref="A1:X24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2190,142 +1992,140 @@
   <sheetData>
     <row r="1" spans="1:24" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B1" s="12"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="18"/>
-      <c r="M1" s="18"/>
-      <c r="N1" s="18"/>
-      <c r="O1" s="18"/>
-      <c r="P1" s="18"/>
-      <c r="Q1" s="18"/>
-      <c r="R1" s="18"/>
-      <c r="S1" s="18"/>
-      <c r="T1" s="18"/>
-      <c r="U1" s="18"/>
-      <c r="V1" s="18"/>
-      <c r="W1" s="18"/>
-      <c r="X1" s="18"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
+      <c r="L1" s="23"/>
+      <c r="M1" s="23"/>
+      <c r="N1" s="23"/>
+      <c r="O1" s="23"/>
+      <c r="P1" s="23"/>
+      <c r="Q1" s="23"/>
+      <c r="R1" s="23"/>
+      <c r="S1" s="23"/>
+      <c r="T1" s="23"/>
+      <c r="U1" s="23"/>
+      <c r="V1" s="23"/>
+      <c r="W1" s="23"/>
+      <c r="X1" s="23"/>
     </row>
     <row r="2" spans="1:24" ht="32.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="B2" s="5"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
-      <c r="I2" s="18"/>
-      <c r="J2" s="18"/>
-      <c r="K2" s="18"/>
-      <c r="L2" s="18"/>
-      <c r="M2" s="18"/>
-      <c r="N2" s="18"/>
-      <c r="O2" s="18"/>
-      <c r="P2" s="18"/>
-      <c r="Q2" s="18"/>
-      <c r="R2" s="18"/>
-      <c r="S2" s="18"/>
-      <c r="T2" s="18"/>
-      <c r="U2" s="18"/>
-      <c r="V2" s="18"/>
-      <c r="W2" s="18"/>
-      <c r="X2" s="18"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="23"/>
+      <c r="K2" s="23"/>
+      <c r="L2" s="23"/>
+      <c r="M2" s="23"/>
+      <c r="N2" s="23"/>
+      <c r="O2" s="23"/>
+      <c r="P2" s="23"/>
+      <c r="Q2" s="23"/>
+      <c r="R2" s="23"/>
+      <c r="S2" s="23"/>
+      <c r="T2" s="23"/>
+      <c r="U2" s="23"/>
+      <c r="V2" s="23"/>
+      <c r="W2" s="23"/>
+      <c r="X2" s="23"/>
     </row>
     <row r="3" spans="1:24" ht="32.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
-        <v>17</v>
-      </c>
+      <c r="A3" s="5"/>
       <c r="B3" s="5"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="18"/>
-      <c r="I3" s="18"/>
-      <c r="J3" s="18"/>
-      <c r="K3" s="18"/>
-      <c r="L3" s="18"/>
-      <c r="M3" s="18"/>
-      <c r="N3" s="18"/>
-      <c r="O3" s="18"/>
-      <c r="P3" s="18"/>
-      <c r="Q3" s="18"/>
-      <c r="R3" s="18"/>
-      <c r="S3" s="18"/>
-      <c r="T3" s="18"/>
-      <c r="U3" s="18"/>
-      <c r="V3" s="18"/>
-      <c r="W3" s="18"/>
-      <c r="X3" s="18"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
+      <c r="I3" s="23"/>
+      <c r="J3" s="23"/>
+      <c r="K3" s="23"/>
+      <c r="L3" s="23"/>
+      <c r="M3" s="23"/>
+      <c r="N3" s="23"/>
+      <c r="O3" s="23"/>
+      <c r="P3" s="23"/>
+      <c r="Q3" s="23"/>
+      <c r="R3" s="23"/>
+      <c r="S3" s="23"/>
+      <c r="T3" s="23"/>
+      <c r="U3" s="23"/>
+      <c r="V3" s="23"/>
+      <c r="W3" s="23"/>
+      <c r="X3" s="23"/>
     </row>
     <row r="4" spans="1:24" ht="147" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="18"/>
-      <c r="H4" s="18"/>
-      <c r="I4" s="18"/>
-      <c r="J4" s="18"/>
-      <c r="K4" s="18"/>
-      <c r="L4" s="18"/>
-      <c r="M4" s="18"/>
-      <c r="N4" s="18"/>
-      <c r="O4" s="18"/>
-      <c r="P4" s="18"/>
-      <c r="Q4" s="18"/>
-      <c r="R4" s="18"/>
-      <c r="S4" s="18"/>
-      <c r="T4" s="18"/>
-      <c r="U4" s="18"/>
-      <c r="V4" s="18"/>
-      <c r="W4" s="18"/>
-      <c r="X4" s="18"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="23"/>
+      <c r="I4" s="23"/>
+      <c r="J4" s="23"/>
+      <c r="K4" s="23"/>
+      <c r="L4" s="23"/>
+      <c r="M4" s="23"/>
+      <c r="N4" s="23"/>
+      <c r="O4" s="23"/>
+      <c r="P4" s="23"/>
+      <c r="Q4" s="23"/>
+      <c r="R4" s="23"/>
+      <c r="S4" s="23"/>
+      <c r="T4" s="23"/>
+      <c r="U4" s="23"/>
+      <c r="V4" s="23"/>
+      <c r="W4" s="23"/>
+      <c r="X4" s="23"/>
     </row>
     <row r="5" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="C5" s="6" t="s">
+      <c r="D5" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="E5" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="F5" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="G5" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="F5" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="G5" s="6" t="s">
+      <c r="H5" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="I5" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="I5" s="6" t="s">
+      <c r="J5" s="6" t="s">
         <v>28</v>
-      </c>
-      <c r="J5" s="6" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:24" ht="29.1" customHeight="1" x14ac:dyDescent="0.35">
@@ -2346,13 +2146,13 @@
       </c>
       <c r="G6" s="2"/>
       <c r="H6" s="14" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:24" ht="27.95" customHeight="1" x14ac:dyDescent="0.35">
@@ -2375,7 +2175,7 @@
       <c r="H7" s="14"/>
       <c r="I7" s="2"/>
       <c r="J7" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:24" ht="29.1" customHeight="1" x14ac:dyDescent="0.35">
@@ -2391,14 +2191,14 @@
         <v>43652</v>
       </c>
       <c r="F8" s="11">
-        <f t="shared" ref="F7:F24" si="0">(E8-D8)</f>
+        <f t="shared" ref="F8:F24" si="0">(E8-D8)</f>
         <v>1</v>
       </c>
       <c r="G8" s="2"/>
       <c r="H8" s="14"/>
       <c r="I8" s="2"/>
       <c r="J8" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:24" ht="29.1" customHeight="1" x14ac:dyDescent="0.35">
@@ -2421,7 +2221,7 @@
       <c r="H9" s="14"/>
       <c r="I9" s="2"/>
       <c r="J9" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:24" ht="27.95" customHeight="1" x14ac:dyDescent="0.35">
@@ -2444,7 +2244,7 @@
       <c r="H10" s="14"/>
       <c r="I10" s="2"/>
       <c r="J10" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.35">
@@ -2467,7 +2267,7 @@
       <c r="H11" s="14"/>
       <c r="I11" s="2"/>
       <c r="J11" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:24" ht="29.1" customHeight="1" x14ac:dyDescent="0.35">
@@ -2488,11 +2288,11 @@
       </c>
       <c r="G12" s="2"/>
       <c r="H12" s="14" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="I12" s="2"/>
       <c r="J12" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.35">
@@ -2515,7 +2315,7 @@
       <c r="H13" s="14"/>
       <c r="I13" s="2"/>
       <c r="J13" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:24" ht="29.1" customHeight="1" x14ac:dyDescent="0.35">
@@ -2536,11 +2336,11 @@
       </c>
       <c r="G14" s="2"/>
       <c r="H14" s="15" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I14" s="2"/>
       <c r="J14" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:24" ht="29.1" customHeight="1" x14ac:dyDescent="0.35">
@@ -2561,11 +2361,11 @@
       </c>
       <c r="G15" s="2"/>
       <c r="H15" s="15" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="I15" s="2"/>
       <c r="J15" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.35">
@@ -2588,7 +2388,7 @@
       <c r="H16" s="14"/>
       <c r="I16" s="2"/>
       <c r="J16" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
@@ -2611,7 +2411,7 @@
       <c r="H17" s="14"/>
       <c r="I17" s="2"/>
       <c r="J17" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.35">
@@ -2634,7 +2434,7 @@
       <c r="H18" s="14"/>
       <c r="I18" s="2"/>
       <c r="J18" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="29.1" customHeight="1" x14ac:dyDescent="0.35">
@@ -2657,7 +2457,7 @@
       <c r="H19" s="14"/>
       <c r="I19" s="2"/>
       <c r="J19" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="29.1" customHeight="1" x14ac:dyDescent="0.35">
@@ -2676,11 +2476,13 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G20" s="2"/>
+      <c r="G20" s="2">
+        <v>80</v>
+      </c>
       <c r="H20" s="14"/>
       <c r="I20" s="2"/>
       <c r="J20" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.35">
@@ -2703,7 +2505,7 @@
       <c r="H21" s="14"/>
       <c r="I21" s="2"/>
       <c r="J21" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="29.1" customHeight="1" x14ac:dyDescent="0.35">
@@ -2722,16 +2524,18 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G22" s="2"/>
+      <c r="G22" s="2">
+        <v>85</v>
+      </c>
       <c r="H22" s="14"/>
       <c r="I22" s="2"/>
       <c r="J22" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="29.1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B23" s="4"/>
       <c r="C23" s="2"/>
@@ -2745,36 +2549,40 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G23" s="1"/>
+      <c r="G23" s="1">
+        <v>90</v>
+      </c>
       <c r="H23" s="16"/>
       <c r="I23" s="1"/>
       <c r="J23" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A24" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="B24" s="19"/>
-      <c r="C24" s="20"/>
-      <c r="D24" s="21">
+      <c r="A24" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="B24" s="18"/>
+      <c r="C24" s="19"/>
+      <c r="D24" s="20">
         <v>43763</v>
       </c>
-      <c r="E24" s="21">
+      <c r="E24" s="20">
         <v>43764</v>
       </c>
-      <c r="F24" s="22">
+      <c r="F24" s="21">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G24" s="20"/>
-      <c r="H24" s="23" t="s">
-        <v>33</v>
-      </c>
-      <c r="I24" s="20"/>
+      <c r="G24" s="19">
+        <v>100</v>
+      </c>
+      <c r="H24" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="I24" s="19"/>
       <c r="J24" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>